<commit_message>
nvelle base des variables Olivier
</commit_message>
<xml_diff>
--- a/data/variables REGION.xlsx
+++ b/data/variables REGION.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noack\gitCereq\cereq-dataviz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8EF5CE-B229-4530-AC8B-47115E24AB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CCE262-5286-4BAF-A58B-62AA5B0A7D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC812408-9A77-4928-8217-C3B54F3B835A}"/>
+    <workbookView xWindow="-19320" yWindow="360" windowWidth="19440" windowHeight="15000" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,84 +36,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Ordre_menu1</t>
   </si>
   <si>
+    <t>Nom_colonne</t>
+  </si>
+  <si>
+    <t>Titre_graphique</t>
+  </si>
+  <si>
+    <t>Bulle</t>
+  </si>
+  <si>
+    <t>taux_emploi</t>
+  </si>
+  <si>
+    <t>part_chomage</t>
+  </si>
+  <si>
+    <t>taux_chomage</t>
+  </si>
+  <si>
+    <t>Le taux de chômage correspond à la part des  individus sans emploi et à la recherche d'un emploi parmi les actifs (individus en emploi ou au chômage)</t>
+  </si>
+  <si>
+    <t>taux_edi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion d'individus en emploi non-salarié (personne à son compte ou aide familial), en contrat à durée indéterminée (CDI) ou avec le statut de fonctionnaire </t>
+  </si>
+  <si>
+    <t>revenu_travail</t>
+  </si>
+  <si>
+    <t>Niveau de salaire ou traitement mensuel net primes incluses médian. Le revenu médian est la valeur telle que la moitié des individus de la population considérée gagne plus, l'autre moitié gagne  moins.</t>
+  </si>
+  <si>
+    <t>pos_cadres</t>
+  </si>
+  <si>
+    <t>pos_prof_inter</t>
+  </si>
+  <si>
+    <t>pos_emp_ouv_q</t>
+  </si>
+  <si>
+    <t>pos_emp_ouv_nq</t>
+  </si>
+  <si>
+    <t>traj_1</t>
+  </si>
+  <si>
+    <t>traj_2</t>
+  </si>
+  <si>
+    <t>traj_3</t>
+  </si>
+  <si>
+    <t>traj_7</t>
+  </si>
+  <si>
     <t>Ordre_menu2</t>
   </si>
   <si>
-    <t>Nom_colonne</t>
-  </si>
-  <si>
-    <t>Titre_graphique</t>
-  </si>
-  <si>
-    <t>Bulle</t>
-  </si>
-  <si>
-    <t>taux_emploi</t>
-  </si>
-  <si>
-    <t>Taux d’emploi à trois ans</t>
-  </si>
-  <si>
-    <t>part_chomage</t>
-  </si>
-  <si>
-    <t>Proportion de sortants au chômage à trois ans</t>
-  </si>
-  <si>
-    <t>taux_chomage</t>
-  </si>
-  <si>
-    <t>Taux de chômage à trois ans</t>
-  </si>
-  <si>
-    <t>Le taux de chômage correspond à la part des  individus sans emploi et à la recherche d'un emploi parmi les actifs (individus en emploi ou au chômage)</t>
-  </si>
-  <si>
-    <t>traj_1</t>
-  </si>
-  <si>
-    <t>Cette information résulte d'une typologie des trajectoires construite par le Céreq par des méthodes statistiques.</t>
-  </si>
-  <si>
-    <t>traj_2</t>
-  </si>
-  <si>
-    <t>traj_3</t>
-  </si>
-  <si>
-    <t>traj_7</t>
-  </si>
-  <si>
-    <t>taux_edi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proportion d'individus en emploi non-salarié (personne à son compte ou aide familial), en contrat à durée indéterminée (CDI) ou avec le statut de fonctionnaire </t>
-  </si>
-  <si>
-    <t>revenu_travail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenu mensuel médian à trois ans </t>
-  </si>
-  <si>
-    <t>pos_cadres</t>
-  </si>
-  <si>
-    <t>Proportion de sortants cadres à trois ans</t>
-  </si>
-  <si>
-    <t>pos_prof_inter</t>
-  </si>
-  <si>
-    <t>pos_emp_ouv_q</t>
-  </si>
-  <si>
-    <t>pos_emp_ouv_nq</t>
+    <t>Diplôme de l'enseignement secondaire</t>
+  </si>
+  <si>
+    <t>Diplôme de l'enseignement supérieur court</t>
+  </si>
+  <si>
+    <t>Diplôme de l'enseignement supérieur long</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes ayant connu un accès rapide à l’emploi durable à l'emploi à durée indéterminée</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes ayant connu un accès différé à l’emploi à durée indéterminée</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes ayant connu un accès rapide et récurrent à l’emploi à durée déterminée</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes ayant connu un chômage persistant ou récurrent</t>
+  </si>
+  <si>
+    <t>En octobre 2020, trois années après la fin de formation initiale</t>
+  </si>
+  <si>
+    <t>Taux d’emploi en octobre 2020</t>
+  </si>
+  <si>
+    <t>Taux de chômage en octobre 2020</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes au chômage en octobre 2020</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes en emploi à durée indéterminée en octobre 2020</t>
+  </si>
+  <si>
+    <t>Revenu mensuel médian en octobre 2020</t>
+  </si>
+  <si>
+    <t>Proportion de sortants professions intermédiaires en octobre 2020</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes employés ou ouvriers qualifiés en octobre 2020</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes employés ou ouvriers peu qualifiés en octobre 2020</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes cadres en octobre 2020</t>
+  </si>
+  <si>
+    <t>Non-diplômés</t>
   </si>
   <si>
     <t>nondiplome</t>
@@ -128,50 +167,17 @@
     <t>superieur_long</t>
   </si>
   <si>
-    <t>Aucun diplôme</t>
-  </si>
-  <si>
-    <t>Diplôme du secondaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diplôme de l'enseignement supérieur court </t>
-  </si>
-  <si>
-    <t>Diplôme de l'enseignement supérieur long</t>
-  </si>
-  <si>
-    <t>Niveau de salaire ou traitement mensuel net primes incluses médian. Le revenu médian est la valeur telle que la moitié des individus de la population considérée gagne plus, l'autre moitié gagne moins.</t>
-  </si>
-  <si>
-    <t>Proportion de sortants ayant connu un accès rapide à l’emploi durable</t>
-  </si>
-  <si>
-    <t>Proportion de sortants ayant connu un accès différé à l’emploi durable</t>
-  </si>
-  <si>
-    <t>Proportion de sortants ayant connu une succession d'emplois courts</t>
-  </si>
-  <si>
-    <t>Proportion de sortants ayant connu un chômage persistant ou récurrent</t>
-  </si>
-  <si>
-    <t>Proportion de sortants en emploi à durée indéterminé à trois ans</t>
-  </si>
-  <si>
-    <t>Proportion de sortants professions intermédiaires à trois ans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proportion de sortants employés ou ouvriers qualifiés à trois ans  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proportion de sortants employés ou ouvriers non qualifiés à trois ans  </t>
+    <t>pos_autres</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes occupant un emploi dans une autre catégorie de professions en octobre 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,23 +186,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="MS Sans Serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,21 +240,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,299 +573,255 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C3281A-5991-4134-B1E0-04DFFC2A4C32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCC49D9-688F-41A5-BE55-128E36F0155B}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="126.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>35</v>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>36</v>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1">
-        <v>2</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1">
-        <v>4</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1075,8 +1057,19 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3559f96-a391-4298-a476-5fa029e2109e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE4516A5-532D-4F33-ABBA-648E1D6B0D7B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DD558F8-9C61-4625-9943-A9AFF41A0CEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1095,9 +1088,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00D316AA-8FBD-4DFF-9CD0-DF4460B884C6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
+    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
modif base avec olivier
</commit_message>
<xml_diff>
--- a/data/variables REGION.xlsx
+++ b/data/variables REGION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noack\gitCereq\cereq-dataviz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2064D36-84D1-4636-B097-6DA0C5715A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B03812-8456-4284-96AA-CD28BBAAB1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Diplôme de l'enseignement supérieur long</t>
   </si>
   <si>
-    <t>Proportion de jeunes ayant connu un accès rapide à l’emploi durable à l'emploi à durée indéterminée</t>
-  </si>
-  <si>
     <t>Proportion de jeunes ayant connu un accès différé à l’emploi à durée indéterminée</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Proportion de jeunes occupant un emploi dans une autre catégorie de professions en octobre 2020</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes ayant connu un accès rapide et durable à l'emploi à durée indéterminée</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -614,10 +614,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -653,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
@@ -667,7 +667,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -681,7 +681,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -714,15 +714,15 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="2"/>
@@ -735,7 +735,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -746,7 +746,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -757,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -768,7 +768,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -776,10 +776,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -787,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>21</v>
@@ -798,7 +798,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>22</v>
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>23</v>
@@ -823,6 +823,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
@@ -831,15 +840,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1066,20 +1066,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
     <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>